<commit_message>
India Mean Temperature With linear regression
Random split no Fold
</commit_message>
<xml_diff>
--- a/datatabt_3.xlsx
+++ b/datatabt_3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mustafasoydan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DFBF8F-CFE5-094F-8D96-B1D1B4878D77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8B492D5-8830-1A4E-A504-1D9895CCDE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14700" yWindow="740" windowWidth="14700" windowHeight="17220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -435,7 +435,7 @@
   <dimension ref="A1:F1461"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>